<commit_message>
data sheet execute handled
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Automate_automation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E138B11-8CEF-4167-9EBB-F5EEF78718EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280139D7-7169-4A74-BA7F-01458E98161B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
   <si>
     <t>TC01</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>OpenUrl</t>
+  </si>
+  <si>
+    <t>execute</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9B3BAF-3AC2-4D45-A37B-B97542CB345B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -975,9 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D275F10-6298-43A3-A67C-7C0A5C364352}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -986,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
@@ -1032,7 +1033,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
added flags in excel
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Automate_automation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280139D7-7169-4A74-BA7F-01458E98161B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D787A60-FA0B-4B6B-A05C-97F0A334ED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
   <si>
     <t>TC01</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>execute</t>
+  </si>
+  <si>
+    <t>HeadLess</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>GetPassScreenshot</t>
   </si>
 </sst>
 </file>
@@ -606,236 +618,267 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
-    <col min="10" max="10" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.90625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" customWidth="1"/>
+    <col min="11" max="11" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" t="e">
-        <f>CONCATENATE(B2,"_",#REF!,"_",C2,"_",D2)</f>
+      <c r="F2" t="e">
+        <f>CONCATENATE(C2,"_",#REF!,"_",D2,"_",E2)</f>
         <v>#REF!</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="e">
-        <f>CONCATENATE(B4,"_",#REF!,"_",C4,"_",D4)</f>
+      <c r="F4" t="e">
+        <f>CONCATENATE(C4,"_",#REF!,"_",D4,"_",E4)</f>
         <v>#REF!</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="e">
-        <f>CONCATENATE(B5,"_",#REF!,"_",C5,"_",D5)</f>
+      <c r="F5" t="e">
+        <f>CONCATENATE(C5,"_",#REF!,"_",D5,"_",E5)</f>
         <v>#REF!</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
       <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>56</v>
       </c>
-      <c r="E7" t="e">
-        <f>CONCATENATE(B7,"_",#REF!,"_",C7,"_",D7)</f>
+      <c r="F7" t="e">
+        <f>CONCATENATE(C7,"_",#REF!,"_",D7,"_",E7)</f>
         <v>#REF!</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
       <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="e">
-        <f>CONCATENATE(B8,"_",#REF!,"_",C8,"_",D8)</f>
+      <c r="F8" t="e">
+        <f>CONCATENATE(C8,"_",#REF!,"_",D8,"_",E8)</f>
         <v>#REF!</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
       <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -849,7 +892,7 @@
           <x14:formula1>
             <xm:f>CommonSheet!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F12 F2:F10</xm:sqref>
+          <xm:sqref>G12 G2:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -976,219 +1019,249 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D275F10-6298-43A3-A67C-7C0A5C364352}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>61</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>38</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>47</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new columns in report, changed log formation
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Automate_automation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Selenium_Python-KeywordBased_Framework\keyword_based_automation_framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D787A60-FA0B-4B6B-A05C-97F0A334ED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7799037D-B616-4BC7-9F23-9F089CC16AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
@@ -620,9 +620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:B10"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,6 +702,15 @@
       <c r="G2" t="s">
         <v>60</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>111</v>
+      </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
@@ -724,6 +733,15 @@
       </c>
       <c r="G3" t="s">
         <v>58</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -749,6 +767,15 @@
       <c r="G4" t="s">
         <v>58</v>
       </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>333</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -772,6 +799,15 @@
       </c>
       <c r="G5" t="s">
         <v>58</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>44</v>
+      </c>
+      <c r="J5">
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
primary setup bat and component concept added
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Selenium_Python-KeywordBased_Framework\keyword_based_automation_framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7799037D-B616-4BC7-9F23-9F089CC16AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAA69FC-0452-40FA-979A-983756A78EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
     <sheet name="DriverSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="CommonSheet" sheetId="3" r:id="rId3"/>
-    <sheet name="DataSheet" sheetId="5" r:id="rId4"/>
+    <sheet name="Components" sheetId="6" r:id="rId3"/>
+    <sheet name="CommonSheet" sheetId="3" r:id="rId4"/>
+    <sheet name="DataSheet" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
   <si>
     <t>TC01</t>
   </si>
@@ -234,6 +235,15 @@
   </si>
   <si>
     <t>GetPassScreenshot</t>
+  </si>
+  <si>
+    <t>CompomentName</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>ComponentName</t>
   </si>
 </sst>
 </file>
@@ -297,10 +307,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,11 +631,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,18 +643,19 @@
     <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.453125" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.90625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" customWidth="1"/>
-    <col min="11" max="11" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.90625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" customWidth="1"/>
+    <col min="12" max="12" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -652,34 +666,37 @@
         <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -690,32 +707,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" t="e">
-        <f>CONCATENATE(C2,"_",#REF!,"_",D2,"_",E2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>11</v>
-      </c>
-      <c r="J2">
-        <v>111</v>
-      </c>
-      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -725,92 +723,83 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="e">
+        <f>CONCATENATE(C4,"_",#REF!,"_",E4,"_",F4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>222</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="e">
-        <f>CONCATENATE(C4,"_",#REF!,"_",D4,"_",E4)</f>
+      <c r="G5" t="e">
+        <f>CONCATENATE(C5,"_",#REF!,"_",E5,"_",F5)</f>
         <v>#REF!</v>
       </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4">
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I4">
+      <c r="J5">
         <v>33</v>
       </c>
-      <c r="J4">
+      <c r="K5">
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="e">
-        <f>CONCATENATE(C5,"_",#REF!,"_",D5,"_",E5)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>44</v>
-      </c>
-      <c r="J5">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -818,18 +807,30 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>44</v>
+      </c>
+      <c r="K6">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -837,85 +838,23 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
       <c r="E7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" t="e">
-        <f>CONCATENATE(C7,"_",#REF!,"_",D7,"_",E7)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="e">
-        <f>CONCATENATE(C8,"_",#REF!,"_",D8,"_",E8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <v>11</v>
       </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
+      <c r="K7">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +867,7 @@
           <x14:formula1>
             <xm:f>CommonSheet!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>G12 G2:G10</xm:sqref>
+          <xm:sqref>H12 H2:H7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -937,6 +876,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE84D76C-E735-41F7-8798-6801FDF7EF22}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>55</v>
+      </c>
+      <c r="G2">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>66</v>
+      </c>
+      <c r="G3">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>77</v>
+      </c>
+      <c r="G4">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>88</v>
+      </c>
+      <c r="G5">
+        <v>888</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{1341A0AB-1E91-4633-A6F1-B0C02B7BA1F9}">
+          <x14:formula1>
+            <xm:f>CommonSheet!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9B3BAF-3AC2-4D45-A37B-B97542CB345B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1053,7 +1139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D275F10-6298-43A3-A67C-7C0A5C364352}">
   <dimension ref="A1:H9"/>
   <sheetViews>

</xml_diff>

<commit_message>
added a custom function
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Selenium_Python-KeywordBased_Framework\keyword_based_automation_framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E8FC99-3A99-42F8-8CBA-E30425F061B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F5617-CE43-4001-9910-F846CAE03441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
   <si>
     <t>TC01</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Profile</t>
   </si>
   <si>
-    <t>TC02</t>
-  </si>
-  <si>
     <t>https://automationintesting.com/selenium/testpage</t>
   </si>
   <si>
@@ -129,84 +126,18 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>DataSheet!B2:DataSheet!B3</t>
-  </si>
-  <si>
     <t>test1</t>
   </si>
   <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>test7</t>
-  </si>
-  <si>
-    <t>test8</t>
-  </si>
-  <si>
     <t>testlast1</t>
   </si>
   <si>
-    <t>testlast2</t>
-  </si>
-  <si>
-    <t>testlast3</t>
-  </si>
-  <si>
-    <t>testlast4</t>
-  </si>
-  <si>
-    <t>testlast5</t>
-  </si>
-  <si>
-    <t>testlast6</t>
-  </si>
-  <si>
-    <t>testlast7</t>
-  </si>
-  <si>
-    <t>testlast8</t>
-  </si>
-  <si>
     <t>testfirst1</t>
   </si>
   <si>
     <t>testfirst2</t>
   </si>
   <si>
-    <t>testfirst3</t>
-  </si>
-  <si>
-    <t>testfirst4</t>
-  </si>
-  <si>
-    <t>testfirst5</t>
-  </si>
-  <si>
-    <t>testfirst6</t>
-  </si>
-  <si>
-    <t>testfirst7</t>
-  </si>
-  <si>
-    <t>testfirst8</t>
-  </si>
-  <si>
     <t>app_url</t>
   </si>
   <si>
@@ -228,9 +159,6 @@
     <t>HeadLess</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -250,6 +178,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Dashboard_page</t>
+  </si>
+  <si>
+    <t>DataSheet!B3:DataSheet!B3</t>
   </si>
 </sst>
 </file>
@@ -313,10 +250,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,11 +577,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,19 +606,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -687,19 +627,19 @@
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -713,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -729,11 +669,8 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
+      <c r="D3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -741,126 +678,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" t="e">
-        <f>CONCATENATE(C4,"_",#REF!,"_",E4,"_",F4)</f>
-        <v>#REF!</v>
-      </c>
       <c r="H4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>222</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="e">
-        <f>CONCATENATE(C5,"_",#REF!,"_",E5,"_",F5)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>33</v>
-      </c>
-      <c r="K5">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>44</v>
-      </c>
-      <c r="K6">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>11</v>
-      </c>
-      <c r="K7">
-        <v>111</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -873,7 +700,7 @@
           <x14:formula1>
             <xm:f>CommonSheet!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H12 H2:H7</xm:sqref>
+          <xm:sqref>H8 H4 H2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B8E16411-152E-427B-96C2-6BE5097C058D}">
           <x14:formula1>
@@ -889,15 +716,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE84D76C-E735-41F7-8798-6801FDF7EF22}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.26953125" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
@@ -906,116 +734,117 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>55</v>
-      </c>
-      <c r="G2">
-        <v>555</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3">
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="F3">
-        <v>66</v>
-      </c>
-      <c r="G3">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>77</v>
-      </c>
-      <c r="G4">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>88</v>
-      </c>
-      <c r="G5">
-        <v>888</v>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A4:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1024,15 +853,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C39FD7D-EFCE-457A-96D3-6B1E78C265BF}">
           <x14:formula1>
-            <xm:f>CommonSheet!$F$2:$F$45</xm:f>
+            <xm:f>CommonSheet!$E$2:$E$45</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D262</xm:sqref>
+          <xm:sqref>D2:D260</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{199F2882-2E4A-4AD3-A747-2AFF75D80E00}">
           <x14:formula1>
             <xm:f>CommonSheet!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B14</xm:sqref>
+          <xm:sqref>B2:B12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1042,10 +871,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9B3BAF-3AC2-4D45-A37B-B97542CB345B}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1054,100 +883,99 @@
     <col min="2" max="2" width="25.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7265625" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1158,10 +986,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D275F10-6298-43A3-A67C-7C0A5C364352}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1172,25 +1000,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -1201,25 +1029,25 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1227,181 +1055,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zoom in ad out custom function added
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Selenium_Python-KeywordBased_Framework\keyword_based_automation_framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F5617-CE43-4001-9910-F846CAE03441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD0BB00-313C-4A1A-A576-77BC46167585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="51">
   <si>
     <t>TC01</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>DataSheet!B3:DataSheet!B3</t>
+  </si>
+  <si>
+    <t>custom-zoomin</t>
   </si>
 </sst>
 </file>
@@ -716,10 +719,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE84D76C-E735-41F7-8798-6801FDF7EF22}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,11 +814,8 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -824,7 +824,7 @@
         <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
@@ -836,15 +836,27 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A4:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -855,13 +867,13 @@
           <x14:formula1>
             <xm:f>CommonSheet!$E$2:$E$45</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D260</xm:sqref>
+          <xm:sqref>D2:D261</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{199F2882-2E4A-4AD3-A747-2AFF75D80E00}">
           <x14:formula1>
             <xm:f>CommonSheet!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B12</xm:sqref>
+          <xm:sqref>B2:B13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -873,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9B3BAF-3AC2-4D45-A37B-B97542CB345B}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,6 +983,9 @@
       </c>
       <c r="C6" t="s">
         <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
framework update now playwright introduced as option
</commit_message>
<xml_diff>
--- a/config/testcase_driver_data_sheet.xlsx
+++ b/config/testcase_driver_data_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Selenium_Python-KeywordBased_Framework\keyword_based_automation_framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD0BB00-313C-4A1A-A576-77BC46167585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B196D0D-0741-4208-A5E6-32F5446E44BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="960" windowWidth="14400" windowHeight="9020" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="4" r:id="rId1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE84D76C-E735-41F7-8798-6801FDF7EF22}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9B3BAF-3AC2-4D45-A37B-B97542CB345B}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,7 +917,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -994,6 +994,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{33D281C4-54B2-4CFD-846E-5C053672E4E8}">
+      <formula1>$A:$A</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>